<commit_message>
09/01/2021 move cursor to A1
</commit_message>
<xml_diff>
--- a/tuning/ISAM_Tuning.xlsx
+++ b/tuning/ISAM_Tuning.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/whannon@us.ibm.com/documentation/Am/Performance/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:81_{D3D91B5A-9E12-5349-87B7-9E89FF7074D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:81_{765AB025-E059-A144-A17B-5ED9AD31E7FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,8 +24,8 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <customWorkbookViews>
+    <customWorkbookView name="whannon - Personal View" guid="{428EE15C-FAD5-428C-9A93-0F1E50589A6D}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1916" windowHeight="962" activeSheetId="1"/>
     <customWorkbookView name="William Hannon Jr - Personal View" guid="{340C4338-CA95-6642-AF8A-4D0D155F5409}" mergeInterval="0" personalView="1" maximized="1" yWindow="23" windowWidth="1680" windowHeight="1027" activeSheetId="1"/>
-    <customWorkbookView name="whannon - Personal View" guid="{428EE15C-FAD5-428C-9A93-0F1E50589A6D}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1916" windowHeight="962" activeSheetId="1"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -4453,7 +4453,7 @@
   <userInfo guid="{B2DBF983-6DAB-6F40-A024-447E238D6676}" name="William Hannon Jr" id="-1404499576" dateTime="2020-05-13T14:13:33"/>
   <userInfo guid="{B2DBF983-6DAB-6F40-A024-447E238D6676}" name="William Hannon Jr" id="-1404482469" dateTime="2020-06-08T12:14:42"/>
   <userInfo guid="{AC9CE79B-8C52-1744-B28F-6E168B04899E}" name="William Hannon Jr" id="-1404494652" dateTime="2021-04-19T11:42:50"/>
-  <userInfo guid="{1E3E9BA8-1B5A-3044-A730-F5D4537C6D24}" name="William Hannon Jr" id="-1404469762" dateTime="2021-09-01T11:33:58"/>
+  <userInfo guid="{1E3E9BA8-1B5A-3044-A730-F5D4537C6D24}" name="William Hannon Jr" id="-1404447978" dateTime="2021-09-01T16:19:23"/>
 </users>
 </file>
 
@@ -4782,7 +4782,7 @@
   <dimension ref="A1:H45"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="E7" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight"/>
@@ -5531,19 +5531,19 @@
   </sheetData>
   <autoFilter ref="B1:H45" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <customSheetViews>
+    <customSheetView guid="{428EE15C-FAD5-428C-9A93-0F1E50589A6D}" showAutoFilter="1">
+      <pane xSplit="4" ySplit="1" topLeftCell="E9" activePane="bottomRight" state="frozen"/>
+      <selection pane="bottomRight" activeCell="E10" sqref="E10"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <pageSetup orientation="portrait" r:id="rId1"/>
+      <autoFilter ref="B1:H40" xr:uid="{0B316F08-FC1A-6F45-9C16-97F971AD0F93}"/>
+    </customSheetView>
     <customSheetView guid="{340C4338-CA95-6642-AF8A-4D0D155F5409}" showAutoFilter="1">
       <pane xSplit="4" ySplit="1" topLeftCell="E17" activePane="bottomRight" state="frozen"/>
       <selection pane="bottomRight" activeCell="E19" sqref="E19"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <pageSetup orientation="portrait" r:id="rId1"/>
-      <autoFilter ref="B1:H45" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
-    </customSheetView>
-    <customSheetView guid="{428EE15C-FAD5-428C-9A93-0F1E50589A6D}" showAutoFilter="1">
-      <pane xSplit="4" ySplit="1" topLeftCell="E9" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="E10" sqref="E10"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId2"/>
-      <autoFilter ref="B1:H40" xr:uid="{80E9F918-3307-CC44-8C46-323B76ED5821}"/>
+      <autoFilter ref="B1:H45" xr:uid="{70F26253-AEA8-ED47-A9B9-D7445E4B6692}"/>
     </customSheetView>
   </customSheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5654,11 +5654,11 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{340C4338-CA95-6642-AF8A-4D0D155F5409}" state="hidden">
+    <customSheetView guid="{428EE15C-FAD5-428C-9A93-0F1E50589A6D}" state="hidden">
       <selection activeCell="D8" sqref="D8"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
-    <customSheetView guid="{428EE15C-FAD5-428C-9A93-0F1E50589A6D}" state="hidden">
+    <customSheetView guid="{340C4338-CA95-6642-AF8A-4D0D155F5409}" state="hidden">
       <selection activeCell="D8" sqref="D8"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
@@ -5672,7 +5672,7 @@
   <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5694,11 +5694,11 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{340C4338-CA95-6642-AF8A-4D0D155F5409}">
+    <customSheetView guid="{428EE15C-FAD5-428C-9A93-0F1E50589A6D}">
       <selection activeCell="B1" sqref="B1"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
-    <customSheetView guid="{428EE15C-FAD5-428C-9A93-0F1E50589A6D}">
+    <customSheetView guid="{340C4338-CA95-6642-AF8A-4D0D155F5409}">
       <selection activeCell="B1" sqref="B1"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>

</xml_diff>

<commit_message>
Internal Database -> where <number> is calculated ( 125 (or lower if impacting LMI)
</commit_message>
<xml_diff>
--- a/tuning/ISAM_Tuning.xlsx
+++ b/tuning/ISAM_Tuning.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10808"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10209"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/whannon@us.ibm.com/documentation/Am/Performance/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/whannon/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:81_{765AB025-E059-A144-A17B-5ED9AD31E7FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:81_{91095BEE-7BEC-774C-9ED1-F17AD625EE8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tuning" sheetId="1" r:id="rId1"/>
@@ -24,8 +24,8 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <customWorkbookViews>
+    <customWorkbookView name="William Hannon Jr - Personal View" guid="{340C4338-CA95-6642-AF8A-4D0D155F5409}" mergeInterval="0" personalView="1" maximized="1" yWindow="23" windowWidth="1680" windowHeight="1027" activeSheetId="1"/>
     <customWorkbookView name="whannon - Personal View" guid="{428EE15C-FAD5-428C-9A93-0F1E50589A6D}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1916" windowHeight="962" activeSheetId="1"/>
-    <customWorkbookView name="William Hannon Jr - Personal View" guid="{340C4338-CA95-6642-AF8A-4D0D155F5409}" mergeInterval="0" personalView="1" maximized="1" yWindow="23" windowWidth="1680" windowHeight="1027" activeSheetId="1"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -524,6 +524,15 @@
     </r>
   </si>
   <si>
+    <t>Sufficient VMWare vmkernel scheduler CPU resources
+Best Practices for Performance Tuning of Latency-Sensitive
+BIOS Power Management settings
+InterruptThrottleRate
+ethernetX.coalescingScheme
+Do not overcommit vCPUs as compared to pCPUs
+Do not overcommit VMWare physical memory</t>
+  </si>
+  <si>
     <r>
       <t xml:space="preserve">isam_cluster.config.connectionManager.agedTimeout = 3600s
 isam_cluster.config.connectionManager.connectionTimeout=20s
@@ -534,11 +543,12 @@
 If external database:
 isam_cluster.config.connectionManager.maxPoolSize= &lt;number&gt;
                                                                                          where &lt;number&gt; is calculated
-                                                                                           ( &lt;External_database_maximum_connections&gt; / number_of_nodes)
+                                                                                           ( &lt;External_database_maximum_connections&gt; / ( number_of_nodes )
                                                                                          Do NOT overcommit maximum connections
 If internal database:
 isam_cluster.config.connectionManager.maxPoolSize= &lt;number&gt;
-                                                                                         where &lt;number&gt; is calculated ( &lt;Maximum_of_128&gt; / number_of_nodes)
+                                                                                         where &lt;number&gt; is calculated ( 125 (or lower if impacting LMI) )
+                                                                                         Do NOT overcommit maximum connections
 isam_cluster.config.connectionManager.minPoolSize=10
 isam_cluster.config.connectionManager.purgePolicy = FailingConnectionOnly
 isam_cluster.config.connectionManager.reapTime = 180s
@@ -556,15 +566,6 @@
       </rPr>
       <t>Remove isam_cluster.config.properties.traceLevel</t>
     </r>
-  </si>
-  <si>
-    <t>Sufficient VMWare vmkernel scheduler CPU resources
-Best Practices for Performance Tuning of Latency-Sensitive
-BIOS Power Management settings
-InterruptThrottleRate
-ethernetX.coalescingScheme
-Do not overcommit vCPUs as compared to pCPUs
-Do not overcommit VMWare physical memory</t>
   </si>
 </sst>
 </file>
@@ -757,7 +758,7 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -766,7 +767,7 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -799,7 +800,7 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -837,7 +838,7 @@
 </file>
 
 <file path=xl/revisions/revisionHeaders.xml><?xml version="1.0" encoding="utf-8"?>
-<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{1E3E9BA8-1B5A-3044-A730-F5D4537C6D24}" diskRevisions="1" revisionId="179" version="68" preserveHistory="9999">
+<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{BA9F6A5A-C856-C141-A363-40E3365320A6}" diskRevisions="1" revisionId="183" version="72" preserveHistory="9999">
   <header guid="{B2AED240-CB75-45B8-8B56-2AD4B49A6DD4}" dateTime="2017-10-13T19:36:07" maxSheetId="3" userName="whannon" r:id="rId1">
     <sheetIdMap count="2">
       <sheetId val="1"/>
@@ -1295,6 +1296,34 @@
     </sheetIdMap>
   </header>
   <header guid="{1E3E9BA8-1B5A-3044-A730-F5D4537C6D24}" dateTime="2021-09-01T14:40:49" maxSheetId="4" userName="William Hannon Jr" r:id="rId68" minRId="179">
+    <sheetIdMap count="3">
+      <sheetId val="1"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{9D2DFEB7-B38B-8E42-B519-582DE0AE2BB8}" dateTime="2025-02-26T11:48:39" maxSheetId="4" userName="William Hannon Jr" r:id="rId69" minRId="180">
+    <sheetIdMap count="3">
+      <sheetId val="1"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{4CADD712-2963-764B-8FFC-9D3CD5D5168D}" dateTime="2025-02-26T12:20:29" maxSheetId="4" userName="William Hannon Jr" r:id="rId70" minRId="181">
+    <sheetIdMap count="3">
+      <sheetId val="1"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{A6A44389-A359-E54A-8E48-E7E1C9B7464B}" dateTime="2025-02-26T14:50:51" maxSheetId="4" userName="William Hannon Jr" r:id="rId71" minRId="182">
+    <sheetIdMap count="3">
+      <sheetId val="1"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{BA9F6A5A-C856-C141-A363-40E3365320A6}" dateTime="2025-02-26T15:09:31" maxSheetId="4" userName="William Hannon Jr" r:id="rId72" minRId="183">
     <sheetIdMap count="3">
       <sheetId val="1"/>
       <sheetId val="2"/>
@@ -4344,6 +4373,86 @@
 </revisions>
 </file>
 
+<file path=xl/revisions/revisionLog69.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="180" sId="1">
+    <oc r="E19" t="inlineStr">
+      <is>
+        <r>
+          <t xml:space="preserve">isam_cluster.config.connectionManager.agedTimeout = 3600s
+isam_cluster.config.connectionManager.connectionTimeout=20s
+                                                                                                  ^^
+                                                                                                  Increase if using GeoIP DB
+isam_cluster.config.connectionManager.enableSharingForDirectLookups = false
+isam_cluster.config.connectionManager.maxIdleTime=300s
+If external database:
+isam_cluster.config.connectionManager.maxPoolSize= &lt;number&gt;
+                                                                                         where &lt;number&gt; is calculated
+                                                                                           ( &lt;External_database_maximum_connections&gt; / number_of_nodes)
+                                                                                         Do NOT overcommit maximum connections
+If internal database:
+isam_cluster.config.connectionManager.maxPoolSize= &lt;number&gt;
+                                                                                         where &lt;number&gt; is calculated ( &lt;Maximum_of_128&gt; / number_of_nodes)
+isam_cluster.config.connectionManager.minPoolSize=10
+isam_cluster.config.connectionManager.purgePolicy = FailingConnectionOnly
+isam_cluster.config.connectionManager.reapTime = 180s
+isam_cluster.config.properties.blockingReadConnectionTimeout = 30s
+isam_cluster.config.properties.traceFile = db2jcc_trace.log
+isam_cluster.config.properties.traceDirectory = /opt/ibm/wlp/usr/servers/default/logs/
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FFC00000"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t>Remove isam_cluster.config.properties.traceLevel</t>
+        </r>
+      </is>
+    </oc>
+    <nc r="E19" t="inlineStr">
+      <is>
+        <r>
+          <t xml:space="preserve">isam_cluster.config.connectionManager.agedTimeout = 3600s
+isam_cluster.config.connectionManager.connectionTimeout=20s
+                                                                                                  ^^
+                                                                                                  Increase if using GeoIP DB
+isam_cluster.config.connectionManager.enableSharingForDirectLookups = false
+isam_cluster.config.connectionManager.maxIdleTime=300s
+If external database:
+isam_cluster.config.connectionManager.maxPoolSize= &lt;number&gt;
+                                                                                         where &lt;number&gt; is calculated
+                                                                                           ( &lt;External_database_maximum_connections&gt; / number_of_nodes)
+                                                                                         Do NOT overcommit maximum connections
+If internal database:
+isam_cluster.config.connectionManager.maxPoolSize= &lt;number&gt;
+                                                                                         where &lt;number&gt; is calculated ( &lt;Maximum_of_128&gt; / number_of_connections_required)
+                                                                                         Do NOT overcommit maximum connections
+isam_cluster.config.connectionManager.minPoolSize=10
+isam_cluster.config.connectionManager.purgePolicy = FailingConnectionOnly
+isam_cluster.config.connectionManager.reapTime = 180s
+isam_cluster.config.properties.blockingReadConnectionTimeout = 30s
+isam_cluster.config.properties.traceFile = db2jcc_trace.log
+isam_cluster.config.properties.traceDirectory = /opt/ibm/wlp/usr/servers/default/logs/
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FFC00000"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t>Remove isam_cluster.config.properties.traceLevel</t>
+        </r>
+      </is>
+    </nc>
+  </rcc>
+</revisions>
+</file>
+
 <file path=xl/revisions/revisionLog7.xml><?xml version="1.0" encoding="utf-8"?>
 <revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <rrc rId="8" sId="2" eol="1" ref="A7:XFD7" action="insertRow"/>
@@ -4387,6 +4496,249 @@
 </revisions>
 </file>
 
+<file path=xl/revisions/revisionLog70.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="181" sId="1">
+    <oc r="E19" t="inlineStr">
+      <is>
+        <r>
+          <t xml:space="preserve">isam_cluster.config.connectionManager.agedTimeout = 3600s
+isam_cluster.config.connectionManager.connectionTimeout=20s
+                                                                                                  ^^
+                                                                                                  Increase if using GeoIP DB
+isam_cluster.config.connectionManager.enableSharingForDirectLookups = false
+isam_cluster.config.connectionManager.maxIdleTime=300s
+If external database:
+isam_cluster.config.connectionManager.maxPoolSize= &lt;number&gt;
+                                                                                         where &lt;number&gt; is calculated
+                                                                                           ( &lt;External_database_maximum_connections&gt; / number_of_nodes)
+                                                                                         Do NOT overcommit maximum connections
+If internal database:
+isam_cluster.config.connectionManager.maxPoolSize= &lt;number&gt;
+                                                                                         where &lt;number&gt; is calculated ( &lt;Maximum_of_128&gt; / number_of_connections_required)
+                                                                                         Do NOT overcommit maximum connections
+isam_cluster.config.connectionManager.minPoolSize=10
+isam_cluster.config.connectionManager.purgePolicy = FailingConnectionOnly
+isam_cluster.config.connectionManager.reapTime = 180s
+isam_cluster.config.properties.blockingReadConnectionTimeout = 30s
+isam_cluster.config.properties.traceFile = db2jcc_trace.log
+isam_cluster.config.properties.traceDirectory = /opt/ibm/wlp/usr/servers/default/logs/
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FFC00000"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t>Remove isam_cluster.config.properties.traceLevel</t>
+        </r>
+      </is>
+    </oc>
+    <nc r="E19" t="inlineStr">
+      <is>
+        <r>
+          <t xml:space="preserve">isam_cluster.config.connectionManager.agedTimeout = 3600s
+isam_cluster.config.connectionManager.connectionTimeout=20s
+                                                                                                  ^^
+                                                                                                  Increase if using GeoIP DB
+isam_cluster.config.connectionManager.enableSharingForDirectLookups = false
+isam_cluster.config.connectionManager.maxIdleTime=300s
+If external database:
+isam_cluster.config.connectionManager.maxPoolSize= &lt;number&gt;
+                                                                                         where &lt;number&gt; is calculated
+                                                                                           ( &lt;External_database_maximum_connections&gt; / number_of_nodes)
+                                                                                         Do NOT overcommit maximum connections ... monitor to avoid overcomiiting
+If internal database:
+isam_cluster.config.connectionManager.maxPoolSize= &lt;number&gt;
+                                                                                         where &lt;number&gt; is calculated ( &lt;Maximum_of_128&gt; / number_of_connections_required)
+                                                                                         Do NOT overcommit maximum connections ... monitor to avoid overcommiting
+isam_cluster.config.connectionManager.minPoolSize=10
+isam_cluster.config.connectionManager.purgePolicy = FailingConnectionOnly
+isam_cluster.config.connectionManager.reapTime = 180s
+isam_cluster.config.properties.blockingReadConnectionTimeout = 30s
+isam_cluster.config.properties.traceFile = db2jcc_trace.log
+isam_cluster.config.properties.traceDirectory = /opt/ibm/wlp/usr/servers/default/logs/
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FFC00000"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t>Remove isam_cluster.config.properties.traceLevel</t>
+        </r>
+      </is>
+    </nc>
+  </rcc>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog71.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="182" sId="1">
+    <oc r="E19" t="inlineStr">
+      <is>
+        <r>
+          <t xml:space="preserve">isam_cluster.config.connectionManager.agedTimeout = 3600s
+isam_cluster.config.connectionManager.connectionTimeout=20s
+                                                                                                  ^^
+                                                                                                  Increase if using GeoIP DB
+isam_cluster.config.connectionManager.enableSharingForDirectLookups = false
+isam_cluster.config.connectionManager.maxIdleTime=300s
+If external database:
+isam_cluster.config.connectionManager.maxPoolSize= &lt;number&gt;
+                                                                                         where &lt;number&gt; is calculated
+                                                                                           ( &lt;External_database_maximum_connections&gt; / number_of_nodes)
+                                                                                         Do NOT overcommit maximum connections ... monitor to avoid overcomiiting
+If internal database:
+isam_cluster.config.connectionManager.maxPoolSize= &lt;number&gt;
+                                                                                         where &lt;number&gt; is calculated ( &lt;Maximum_of_128&gt; / number_of_connections_required)
+                                                                                         Do NOT overcommit maximum connections ... monitor to avoid overcommiting
+isam_cluster.config.connectionManager.minPoolSize=10
+isam_cluster.config.connectionManager.purgePolicy = FailingConnectionOnly
+isam_cluster.config.connectionManager.reapTime = 180s
+isam_cluster.config.properties.blockingReadConnectionTimeout = 30s
+isam_cluster.config.properties.traceFile = db2jcc_trace.log
+isam_cluster.config.properties.traceDirectory = /opt/ibm/wlp/usr/servers/default/logs/
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FFC00000"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t>Remove isam_cluster.config.properties.traceLevel</t>
+        </r>
+      </is>
+    </oc>
+    <nc r="E19" t="inlineStr">
+      <is>
+        <r>
+          <t xml:space="preserve">isam_cluster.config.connectionManager.agedTimeout = 3600s
+isam_cluster.config.connectionManager.connectionTimeout=20s
+                                                                                                  ^^
+                                                                                                  Increase if using GeoIP DB
+isam_cluster.config.connectionManager.enableSharingForDirectLookups = false
+isam_cluster.config.connectionManager.maxIdleTime=300s
+If external database:
+isam_cluster.config.connectionManager.maxPoolSize= &lt;number&gt;
+                                                                                         where &lt;number&gt; is calculated
+                                                                                           ( &lt;External_database_maximum_connections&gt; / ( number_of_nodes * number_of_unique_datasource_ids) )
+                                                                                         Do NOT overcommit maximum connections
+If internal database:
+isam_cluster.config.connectionManager.maxPoolSize= &lt;number&gt;
+                                                                                         where &lt;number&gt; is calculated ( &lt;Maximum_of_128&gt; / number_of_unique_datasource_ids)
+                                                                                         Do NOT overcommit maximum connections
+isam_cluster.config.connectionManager.minPoolSize=10
+isam_cluster.config.connectionManager.purgePolicy = FailingConnectionOnly
+isam_cluster.config.connectionManager.reapTime = 180s
+isam_cluster.config.properties.blockingReadConnectionTimeout = 30s
+isam_cluster.config.properties.traceFile = db2jcc_trace.log
+isam_cluster.config.properties.traceDirectory = /opt/ibm/wlp/usr/servers/default/logs/
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FFC00000"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t>Remove isam_cluster.config.properties.traceLevel</t>
+        </r>
+      </is>
+    </nc>
+  </rcc>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog72.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="183" sId="1">
+    <oc r="E19" t="inlineStr">
+      <is>
+        <r>
+          <t xml:space="preserve">isam_cluster.config.connectionManager.agedTimeout = 3600s
+isam_cluster.config.connectionManager.connectionTimeout=20s
+                                                                                                  ^^
+                                                                                                  Increase if using GeoIP DB
+isam_cluster.config.connectionManager.enableSharingForDirectLookups = false
+isam_cluster.config.connectionManager.maxIdleTime=300s
+If external database:
+isam_cluster.config.connectionManager.maxPoolSize= &lt;number&gt;
+                                                                                         where &lt;number&gt; is calculated
+                                                                                           ( &lt;External_database_maximum_connections&gt; / ( number_of_nodes * number_of_unique_datasource_ids) )
+                                                                                         Do NOT overcommit maximum connections
+If internal database:
+isam_cluster.config.connectionManager.maxPoolSize= &lt;number&gt;
+                                                                                         where &lt;number&gt; is calculated ( &lt;Maximum_of_128&gt; / number_of_unique_datasource_ids)
+                                                                                         Do NOT overcommit maximum connections
+isam_cluster.config.connectionManager.minPoolSize=10
+isam_cluster.config.connectionManager.purgePolicy = FailingConnectionOnly
+isam_cluster.config.connectionManager.reapTime = 180s
+isam_cluster.config.properties.blockingReadConnectionTimeout = 30s
+isam_cluster.config.properties.traceFile = db2jcc_trace.log
+isam_cluster.config.properties.traceDirectory = /opt/ibm/wlp/usr/servers/default/logs/
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FFC00000"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t>Remove isam_cluster.config.properties.traceLevel</t>
+        </r>
+      </is>
+    </oc>
+    <nc r="E19" t="inlineStr">
+      <is>
+        <r>
+          <t xml:space="preserve">isam_cluster.config.connectionManager.agedTimeout = 3600s
+isam_cluster.config.connectionManager.connectionTimeout=20s
+                                                                                                  ^^
+                                                                                                  Increase if using GeoIP DB
+isam_cluster.config.connectionManager.enableSharingForDirectLookups = false
+isam_cluster.config.connectionManager.maxIdleTime=300s
+If external database:
+isam_cluster.config.connectionManager.maxPoolSize= &lt;number&gt;
+                                                                                         where &lt;number&gt; is calculated
+                                                                                           ( &lt;External_database_maximum_connections&gt; / ( number_of_nodes )
+                                                                                         Do NOT overcommit maximum connections
+If internal database:
+isam_cluster.config.connectionManager.maxPoolSize= &lt;number&gt;
+                                                                                         where &lt;number&gt; is calculated ( 125 (or lower if impacting LMI) )
+                                                                                         Do NOT overcommit maximum connections
+isam_cluster.config.connectionManager.minPoolSize=10
+isam_cluster.config.connectionManager.purgePolicy = FailingConnectionOnly
+isam_cluster.config.connectionManager.reapTime = 180s
+isam_cluster.config.properties.blockingReadConnectionTimeout = 30s
+isam_cluster.config.properties.traceFile = db2jcc_trace.log
+isam_cluster.config.properties.traceDirectory = /opt/ibm/wlp/usr/servers/default/logs/
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FFC00000"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t>Remove isam_cluster.config.properties.traceLevel</t>
+        </r>
+      </is>
+    </nc>
+  </rcc>
+</revisions>
+</file>
+
 <file path=xl/revisions/revisionLog8.xml><?xml version="1.0" encoding="utf-8"?>
 <revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <rcc rId="10" sId="1">
@@ -4436,8 +4788,8 @@
 </revisions>
 </file>
 
-<file path=xl/revisions/userNames1.xml><?xml version="1.0" encoding="utf-8"?>
-<users xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" count="16">
+<file path=xl/revisions/userNames.xml><?xml version="1.0" encoding="utf-8"?>
+<users xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" count="17">
   <userInfo guid="{5EBCED96-2F81-4BB0-83BF-42F752F070A1}" name="whannon" id="-336981808" dateTime="2017-10-13T19:36:07"/>
   <userInfo guid="{0FD5F71C-7ADA-4302-BC35-378762EAA384}" name="whannon" id="-336930999" dateTime="2017-11-08T12:53:42"/>
   <userInfo guid="{9AE413E7-4820-4A67-95D2-81FA9633AFC5}" name="whannon" id="-336954853" dateTime="2018-02-08T14:52:55"/>
@@ -4454,13 +4806,14 @@
   <userInfo guid="{B2DBF983-6DAB-6F40-A024-447E238D6676}" name="William Hannon Jr" id="-1404482469" dateTime="2020-06-08T12:14:42"/>
   <userInfo guid="{AC9CE79B-8C52-1744-B28F-6E168B04899E}" name="William Hannon Jr" id="-1404494652" dateTime="2021-04-19T11:42:50"/>
   <userInfo guid="{1E3E9BA8-1B5A-3044-A730-F5D4537C6D24}" name="William Hannon Jr" id="-1404447978" dateTime="2021-09-01T16:19:23"/>
+  <userInfo guid="{BA9F6A5A-C856-C141-A363-40E3365320A6}" name="William Hannon Jr" id="-1404471921" dateTime="2025-02-26T09:17:38"/>
 </users>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -4498,9 +4851,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -4533,26 +4886,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -4585,26 +4921,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -4782,10 +5101,10 @@
   <dimension ref="A1:H45"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="E14" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -4876,7 +5195,7 @@
         <v>73</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G4" s="13" t="str">
         <f>HYPERLINK("https://www.vmware.com/content/dam/digitalmarketing/vmware/en/pdf/techpaper/vmw-tuning-latency-sensitive-workloads-white-paper.pdf", "https://www.vmware.com/content/dam/digitalmarketing/vmware/en/pdf/techpaper/vmw-tuning-latency-sensitive-workloads-white-paper.pdf")</f>
@@ -5121,7 +5440,7 @@
         <v>62</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="F19" s="1" t="s">
         <v>33</v>
@@ -5531,19 +5850,19 @@
   </sheetData>
   <autoFilter ref="B1:H45" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <customSheetViews>
+    <customSheetView guid="{340C4338-CA95-6642-AF8A-4D0D155F5409}" showAutoFilter="1">
+      <pane xSplit="4" ySplit="1" topLeftCell="E17" activePane="bottomRight" state="frozen"/>
+      <selection pane="bottomRight" activeCell="E19" sqref="E19"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <pageSetup orientation="portrait" r:id="rId1"/>
+      <autoFilter ref="B1:H45" xr:uid="{AD555822-8243-3248-8696-EFCE73E08992}"/>
+    </customSheetView>
     <customSheetView guid="{428EE15C-FAD5-428C-9A93-0F1E50589A6D}" showAutoFilter="1">
       <pane xSplit="4" ySplit="1" topLeftCell="E9" activePane="bottomRight" state="frozen"/>
       <selection pane="bottomRight" activeCell="E10" sqref="E10"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <pageSetup orientation="portrait" r:id="rId1"/>
-      <autoFilter ref="B1:H40" xr:uid="{0B316F08-FC1A-6F45-9C16-97F971AD0F93}"/>
-    </customSheetView>
-    <customSheetView guid="{340C4338-CA95-6642-AF8A-4D0D155F5409}" showAutoFilter="1">
-      <pane xSplit="4" ySplit="1" topLeftCell="E17" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="E19" sqref="E19"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId2"/>
-      <autoFilter ref="B1:H45" xr:uid="{70F26253-AEA8-ED47-A9B9-D7445E4B6692}"/>
+      <autoFilter ref="B1:H40" xr:uid="{686D3442-B693-D34A-B6D8-8D20D3D19202}"/>
     </customSheetView>
   </customSheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5654,11 +5973,11 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{428EE15C-FAD5-428C-9A93-0F1E50589A6D}" state="hidden">
+    <customSheetView guid="{340C4338-CA95-6642-AF8A-4D0D155F5409}" state="hidden">
       <selection activeCell="D8" sqref="D8"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
-    <customSheetView guid="{340C4338-CA95-6642-AF8A-4D0D155F5409}" state="hidden">
+    <customSheetView guid="{428EE15C-FAD5-428C-9A93-0F1E50589A6D}" state="hidden">
       <selection activeCell="D8" sqref="D8"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
@@ -5694,11 +6013,11 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{428EE15C-FAD5-428C-9A93-0F1E50589A6D}">
+    <customSheetView guid="{340C4338-CA95-6642-AF8A-4D0D155F5409}">
       <selection activeCell="B1" sqref="B1"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
-    <customSheetView guid="{340C4338-CA95-6642-AF8A-4D0D155F5409}">
+    <customSheetView guid="{428EE15C-FAD5-428C-9A93-0F1E50589A6D}">
       <selection activeCell="B1" sqref="B1"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>

</xml_diff>